<commit_message>
Tested courses to upload
Led to slight modification in doAddClass.  All is well so far.
</commit_message>
<xml_diff>
--- a/TestFiles/coursestoschedule/coursestoscheduleindex.xlsx
+++ b/TestFiles/coursestoschedule/coursestoscheduleindex.xlsx
@@ -36,9 +36,6 @@
     <t>Input is not accepted.  Room label is incorrect on line 1.</t>
   </si>
   <si>
-    <t>Input is not accepted.  Course label is incorrect on line 1.</t>
-  </si>
-  <si>
     <t>Input is not accepted.  Section label is missing on line 5.</t>
   </si>
   <si>
@@ -93,21 +90,6 @@
     <t>Input is not accepted.  Last course exceeds maximum number of hours.</t>
   </si>
   <si>
-    <t>Input is not accepted.  Multiple errors encountered. 0 room size in line 2.  Room capacity below minimum.  Missing section count in line 8. Hours exceeds maximum in line 13.</t>
-  </si>
-  <si>
-    <t>Input is not accepted.  Course name below minimum of 2 characters.</t>
-  </si>
-  <si>
-    <t>Input is not accepted. Course name below minimum of 2 characters.</t>
-  </si>
-  <si>
-    <t>Input is not accepted.  Course name exceeds maximum of 4 characters. Line 6.</t>
-  </si>
-  <si>
-    <t>Input is not accepted. Course name exceeds maximum of 4 characters. Line 11.</t>
-  </si>
-  <si>
     <t>Input is not accepted.  Missing hours specification on line 5 and 9.</t>
   </si>
   <si>
@@ -283,6 +265,24 @@
   </si>
   <si>
     <t>Input is not accepted.  Large file containing an invalid sequence of characters following course numbers.</t>
+  </si>
+  <si>
+    <t>Input is not accepted. Course name below minimum of 2 characters on line 7.</t>
+  </si>
+  <si>
+    <t>Input is not accepted.  Course name below minimum of 2 characters on line 2.</t>
+  </si>
+  <si>
+    <t>Input is not accepted. Course name exceeds maximum of 4 characters on line 11.</t>
+  </si>
+  <si>
+    <t>Input is not accepted.  Course name exceeds maximum of 4 characters on line 6.</t>
+  </si>
+  <si>
+    <t>Input is not accepted.  Multiple errors encountered. 0 room size in line 2.  Room capacity exceeds maximum in line 5.  Missing section count in line 8. Hours exceeds maximum in line 13.</t>
+  </si>
+  <si>
+    <t>Input is not accepted.  Course number is incorrect on line 1.</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,63 +667,63 @@
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
@@ -731,31 +731,31 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>2</v>
@@ -763,95 +763,95 @@
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
@@ -859,79 +859,79 @@
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -939,82 +939,82 @@
     </row>
     <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>